<commit_message>
push all i did during work..
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AFCA43-9555-4296-A72D-618178F02E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="192">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -484,12 +483,6 @@
     <t>basic</t>
   </si>
   <si>
-    <t>ability</t>
-  </si>
-  <si>
-    <t>29 /cd1</t>
-  </si>
-  <si>
     <t>27/cd0</t>
   </si>
   <si>
@@ -505,15 +498,9 @@
     <t>dmg per turn</t>
   </si>
   <si>
-    <t>24/cd2</t>
-  </si>
-  <si>
     <t>heal per turn</t>
   </si>
   <si>
-    <t>bigHeal</t>
-  </si>
-  <si>
     <t>42/cd0</t>
   </si>
   <si>
@@ -563,12 +550,63 @@
   </si>
   <si>
     <t>MID HEAL + HOT</t>
+  </si>
+  <si>
+    <t>ability 3</t>
+  </si>
+  <si>
+    <t>heal reduction</t>
+  </si>
+  <si>
+    <t>ability 1</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>viper sting</t>
+  </si>
+  <si>
+    <t>devotion aura</t>
+  </si>
+  <si>
+    <t>ice block</t>
+  </si>
+  <si>
+    <t>defensive</t>
+  </si>
+  <si>
+    <t>offensive</t>
+  </si>
+  <si>
+    <t>stun/pet target only</t>
+  </si>
+  <si>
+    <t>stun</t>
+  </si>
+  <si>
+    <t>29/cd1</t>
+  </si>
+  <si>
+    <t>28/cd3</t>
+  </si>
+  <si>
+    <t>25/cd2</t>
+  </si>
+  <si>
+    <t>10/cd3</t>
+  </si>
+  <si>
+    <t>purge</t>
+  </si>
+  <si>
+    <t>MULTI-SHOT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -656,10 +694,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -672,12 +716,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -693,9 +734,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -733,7 +774,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -768,23 +809,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -820,26 +844,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1012,50 +1019,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="46.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="10"/>
       <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="8"/>
       <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4"/>
+      <c r="H1" s="8"/>
       <c r="I1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1075,7 +1082,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
@@ -1118,7 +1125,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1141,41 +1148,41 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="10"/>
       <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="10"/>
       <c r="F7" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="3" t="s">
         <v>114</v>
       </c>
       <c r="F8" s="2"/>
@@ -1186,7 +1193,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1199,14 +1206,14 @@
       <c r="E9" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
@@ -1226,7 +1233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1246,44 +1253,44 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="10"/>
       <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="10"/>
       <c r="F13" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="8"/>
       <c r="I13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>166</v>
+      <c r="D14" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>57</v>
@@ -1292,23 +1299,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>52</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
@@ -1324,7 +1331,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -1350,30 +1357,30 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="8"/>
       <c r="C19" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="8"/>
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="H19" s="8"/>
       <c r="I19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
@@ -1393,12 +1400,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>92</v>
@@ -1409,28 +1416,28 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>86</v>
@@ -1445,30 +1452,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="8"/>
       <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="8"/>
       <c r="F25" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="8"/>
       <c r="I25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>99</v>
       </c>
@@ -1476,7 +1483,7 @@
         <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>104</v>
@@ -1491,7 +1498,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>98</v>
       </c>
@@ -1514,7 +1521,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>96</v>
       </c>
@@ -1534,7 +1541,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -1557,30 +1564,30 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="8"/>
       <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="8"/>
       <c r="F31" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="4"/>
+      <c r="H31" s="8"/>
       <c r="I31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
@@ -1600,7 +1607,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -1619,7 +1626,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>125</v>
       </c>
@@ -1635,7 +1642,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="D35" s="1" t="s">
@@ -1647,30 +1654,30 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="8"/>
       <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="8"/>
       <c r="F37" t="s">
         <v>33</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="4"/>
+      <c r="H37" s="8"/>
       <c r="I37" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>57</v>
       </c>
@@ -1690,7 +1697,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
@@ -1710,7 +1717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1730,7 +1737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="D41" s="1"/>
@@ -1742,30 +1749,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="6"/>
+      <c r="B43" s="10"/>
       <c r="C43" t="s">
         <v>149</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="10"/>
       <c r="F43" t="s">
         <v>148</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="4"/>
+      <c r="H43" s="10"/>
       <c r="I43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
@@ -1785,12 +1792,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>144</v>
@@ -1805,12 +1812,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>68</v>
@@ -1825,12 +1832,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>69</v>
@@ -1845,30 +1852,30 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="4"/>
+      <c r="B49" s="8"/>
       <c r="C49" t="s">
         <v>75</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="4"/>
+      <c r="E49" s="8"/>
       <c r="F49" t="s">
         <v>42</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="4"/>
+      <c r="H49" s="8"/>
       <c r="I49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -1884,7 +1891,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>71</v>
       </c>
@@ -1900,9 +1907,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>129</v>
@@ -1912,7 +1919,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="D53" s="1"/>
@@ -1955,52 +1962,83 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A40878C-6B65-4418-BB8F-9DB4DBCC898E}">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>151</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="D1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
         <v>156</v>
       </c>
-      <c r="F1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I1" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H2">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2008,65 +2046,265 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>186</v>
       </c>
       <c r="H3">
         <f>29/2 + 16/2</f>
         <v>22.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="F4">
         <v>13</v>
       </c>
       <c r="H4">
-        <f>13+(13+14+24)/3</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>161</v>
-      </c>
-      <c r="I7" t="s">
+        <f>13+(10+14+25)/3</f>
+        <v>29.333333333333332</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <f>9+(11+14+11+28)/4</f>
+        <v>25</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>19</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
+      <c r="C11" t="s">
+        <v>159</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed bug where team is dead but game doesnt end
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="209">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -249,9 +249,6 @@
     <t>EVISCERATE</t>
   </si>
   <si>
-    <t>CORRUPTION</t>
-  </si>
-  <si>
     <t>damage over time/cc</t>
   </si>
   <si>
@@ -591,9 +588,6 @@
     <t>28/cd3</t>
   </si>
   <si>
-    <t>25/cd2</t>
-  </si>
-  <si>
     <t>10/cd3</t>
   </si>
   <si>
@@ -601,6 +595,63 @@
   </si>
   <si>
     <t>MULTI-SHOT</t>
+  </si>
+  <si>
+    <t>INTERCEPT</t>
+  </si>
+  <si>
+    <t>PET STUN</t>
+  </si>
+  <si>
+    <t>PET AOE</t>
+  </si>
+  <si>
+    <t>CORRUPION</t>
+  </si>
+  <si>
+    <t>DEVOUR MAGIC</t>
+  </si>
+  <si>
+    <t>DEATH COIL</t>
+  </si>
+  <si>
+    <t>STUN AND SELF HEAL</t>
+  </si>
+  <si>
+    <t>UNSTABLE AFFLICTION</t>
+  </si>
+  <si>
+    <t>DOT/STUN AND DMG ON DISPEL</t>
+  </si>
+  <si>
+    <t>SEARING PAIN</t>
+  </si>
+  <si>
+    <t>IMMOLATE</t>
+  </si>
+  <si>
+    <t>DAMAGE + DOT</t>
+  </si>
+  <si>
+    <t>CONFLAGRATE</t>
+  </si>
+  <si>
+    <t>CONSUME IMMOLATE FOR BIG DMG</t>
+  </si>
+  <si>
+    <t>MUST BE SQUISH</t>
+  </si>
+  <si>
+    <t>PET SHOULD DO VERY LITTLE DMG MAYBE 5?</t>
+  </si>
+  <si>
+    <t>13/cd2</t>
+  </si>
+  <si>
+    <t>10/dot</t>
+  </si>
+  <si>
+    <t>20/cd2</t>
   </si>
 </sst>
 </file>
@@ -704,16 +755,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1020,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,26 +1091,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="8"/>
       <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8"/>
+      <c r="E1" s="10"/>
       <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8"/>
+      <c r="H1" s="10"/>
       <c r="I1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1067,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -1076,7 +1127,7 @@
         <v>58</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>65</v>
@@ -1090,39 +1141,39 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>3</v>
+        <v>201</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1133,13 +1184,13 @@
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>30</v>
@@ -1149,48 +1200,48 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="8"/>
       <c r="F7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" t="s">
         <v>131</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1201,16 +1252,16 @@
         <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1227,7 +1278,7 @@
         <v>70</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>3</v>
@@ -1247,50 +1298,50 @@
         <v>55</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="8"/>
       <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="8"/>
       <c r="F13" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="10"/>
       <c r="I13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="D14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>57</v>
@@ -1301,13 +1352,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>52</v>
@@ -1317,26 +1368,30 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
@@ -1348,50 +1403,50 @@
         <v>61</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="I17" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="10"/>
       <c r="C19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="10"/>
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="8"/>
+      <c r="H19" s="10"/>
       <c r="I19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>57</v>
@@ -1402,13 +1457,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>3</v>
@@ -1418,75 +1473,75 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="D23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="10"/>
       <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="10"/>
       <c r="F25" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="8"/>
+      <c r="H25" s="10"/>
       <c r="I25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>3</v>
@@ -1500,45 +1555,45 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="G27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="I27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1549,13 +1604,13 @@
         <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>62</v>
@@ -1565,24 +1620,24 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="8"/>
+      <c r="B31" s="10"/>
       <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="10"/>
       <c r="F31" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="8"/>
+      <c r="H31" s="10"/>
       <c r="I31" t="s">
         <v>38</v>
       </c>
@@ -1615,29 +1670,29 @@
         <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1646,35 +1701,35 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="8"/>
+      <c r="B37" s="10"/>
       <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="10"/>
       <c r="F37" t="s">
         <v>33</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="8"/>
+      <c r="H37" s="10"/>
       <c r="I37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1711,7 +1766,7 @@
         <v>67</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>3</v>
@@ -1750,24 +1805,24 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="10"/>
+      <c r="B43" s="8"/>
       <c r="C43" t="s">
-        <v>149</v>
-      </c>
-      <c r="D43" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="10"/>
+      <c r="E43" s="8"/>
       <c r="F43" t="s">
-        <v>148</v>
-      </c>
-      <c r="G43" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G43" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="10"/>
+      <c r="H43" s="8"/>
       <c r="I43" t="s">
         <v>39</v>
       </c>
@@ -1794,19 +1849,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="G45" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>31</v>
@@ -1814,10 +1869,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>68</v>
@@ -1826,7 +1881,7 @@
         <v>65</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>31</v>
@@ -1834,10 +1889,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>69</v>
@@ -1853,12 +1908,12 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="10"/>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>28</v>
@@ -1867,20 +1922,20 @@
       <c r="F49" t="s">
         <v>42</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G49" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="8"/>
+      <c r="H49" s="10"/>
       <c r="I49" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>74</v>
+        <v>197</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>128</v>
+        <v>198</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>1</v>
@@ -1888,65 +1943,83 @@
       <c r="E50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+      <c r="G50" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>71</v>
+        <v>194</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="G51" s="1" t="s">
-        <v>71</v>
+        <v>200</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>31</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>204</v>
+      </c>
+      <c r="H55" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="G49:H49"/>
@@ -1956,6 +2029,24 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1963,10 +2054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,34 +2072,34 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" t="s">
         <v>154</v>
       </c>
-      <c r="E1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
-        <v>156</v>
-      </c>
       <c r="I1" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -2019,16 +2110,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H2">
         <v>27</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -2046,17 +2137,17 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H3">
         <f>29/2 + 16/2</f>
         <v>22.5</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -2074,20 +2165,20 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="F4">
         <v>13</v>
       </c>
       <c r="H4">
-        <f>13+(10+14+25)/3</f>
-        <v>29.333333333333332</v>
+        <f>13+(10+14+20)/3</f>
+        <v>27.666666666666664</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -2108,10 +2199,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -2121,13 +2212,13 @@
         <v>25</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
@@ -2146,7 +2237,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F6">
         <v>9</v>
@@ -2155,13 +2246,13 @@
         <v>19</v>
       </c>
       <c r="I6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
@@ -2173,7 +2264,28 @@
       <c r="S6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I7" s="6"/>
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <f>9+(0 + 10 + 13 + 10 + 9 +10 + 9)/4</f>
+        <v>24.25</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>177</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -2186,18 +2298,6 @@
       <c r="S7" s="6"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>177</v>
-      </c>
-      <c r="D8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" t="s">
-        <v>175</v>
-      </c>
-      <c r="H8" t="s">
-        <v>157</v>
-      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -2211,12 +2311,6 @@
       <c r="S8" s="6"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>160</v>
-      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -2230,11 +2324,17 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>176</v>
+      </c>
+      <c r="D10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" t="s">
+        <v>156</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -2250,7 +2350,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>159</v>
@@ -2268,6 +2368,12 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -2281,6 +2387,12 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>158</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -2306,6 +2418,32 @@
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
     </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update todolist, chars.xml and add new images
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C459ACF-D13F-43DD-89D6-B15D744D9CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="207">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -240,9 +241,6 @@
     <t>MANA BURN</t>
   </si>
   <si>
-    <t>FEAR</t>
-  </si>
-  <si>
     <t>MUTILATE</t>
   </si>
   <si>
@@ -411,9 +409,6 @@
     <t>DOT</t>
   </si>
   <si>
-    <t>STEAL HP</t>
-  </si>
-  <si>
     <t>cc/lower damage</t>
   </si>
   <si>
@@ -528,9 +523,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>SIPHON LIFE</t>
-  </si>
-  <si>
     <t>REJUVENATION</t>
   </si>
   <si>
@@ -652,12 +644,15 @@
   </si>
   <si>
     <t>20/cd2</t>
+  </si>
+  <si>
+    <t>SEDUCTION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -755,21 +750,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -785,9 +780,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -825,7 +820,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -860,6 +855,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -895,9 +907,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1070,55 +1099,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="10"/>
       <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="8"/>
       <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10"/>
+      <c r="H1" s="8"/>
       <c r="I1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -1127,13 +1156,13 @@
         <v>58</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1141,42 +1170,42 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1184,13 +1213,13 @@
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>30</v>
@@ -1199,52 +1228,52 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="10"/>
       <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="10"/>
       <c r="F7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="8"/>
       <c r="I7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1252,19 +1281,19 @@
         <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
@@ -1278,13 +1307,13 @@
         <v>70</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1298,50 +1327,50 @@
         <v>55</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="10"/>
       <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="10"/>
       <c r="F13" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="8"/>
       <c r="I13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>57</v>
@@ -1350,15 +1379,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>52</v>
@@ -1366,18 +1395,18 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>60</v>
@@ -1386,12 +1415,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
@@ -1403,50 +1432,50 @@
         <v>61</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="I17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="10"/>
+      <c r="B19" s="8"/>
       <c r="C19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="10"/>
+      <c r="E19" s="8"/>
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="10"/>
+      <c r="H19" s="8"/>
       <c r="I19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>57</v>
@@ -1455,15 +1484,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>3</v>
@@ -1471,77 +1500,77 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="8"/>
       <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="8"/>
       <c r="F25" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="10"/>
+      <c r="H25" s="8"/>
       <c r="I25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>3</v>
@@ -1553,50 +1582,50 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="G27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="I27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -1604,13 +1633,13 @@
         <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>62</v>
@@ -1619,30 +1648,30 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="8"/>
       <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="10"/>
+      <c r="E31" s="8"/>
       <c r="F31" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="10"/>
+      <c r="H31" s="8"/>
       <c r="I31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
@@ -1662,7 +1691,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -1670,69 +1699,69 @@
         <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="10"/>
+      <c r="B37" s="8"/>
       <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="10"/>
+      <c r="E37" s="8"/>
       <c r="F37" t="s">
         <v>33</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="10"/>
+      <c r="H37" s="8"/>
       <c r="I37" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>57</v>
       </c>
@@ -1752,9 +1781,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>3</v>
@@ -1766,13 +1795,13 @@
         <v>67</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1780,7 +1809,7 @@
         <v>31</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>3</v>
@@ -1792,7 +1821,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="D41" s="1"/>
@@ -1804,30 +1833,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="10"/>
       <c r="C43" t="s">
-        <v>148</v>
-      </c>
-      <c r="D43" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="8"/>
+      <c r="E43" s="10"/>
       <c r="F43" t="s">
-        <v>147</v>
-      </c>
-      <c r="G43" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G43" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="8"/>
+      <c r="H43" s="10"/>
       <c r="I43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
@@ -1847,32 +1876,32 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>68</v>
@@ -1881,18 +1910,18 @@
         <v>65</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>69</v>
@@ -1907,35 +1936,35 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="10"/>
+      <c r="B49" s="8"/>
       <c r="C49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D49" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="8"/>
+      <c r="E49" s="10"/>
       <c r="F49" t="s">
         <v>42</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="10"/>
+      <c r="H49" s="8"/>
       <c r="I49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>1</v>
@@ -1944,82 +1973,100 @@
         <v>58</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="D53" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>71</v>
+        <v>206</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G55" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H55" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="G49:H49"/>
@@ -2029,80 +2076,62 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="E1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" t="s">
-        <v>155</v>
-      </c>
       <c r="I1" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2110,16 +2139,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H2">
         <v>27</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -2129,7 +2158,7 @@
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2137,17 +2166,17 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H3">
         <f>29/2 + 16/2</f>
         <v>22.5</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -2157,7 +2186,7 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2165,10 +2194,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F4">
         <v>13</v>
@@ -2178,7 +2207,7 @@
         <v>27.666666666666664</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -2191,7 +2220,7 @@
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2199,10 +2228,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -2212,13 +2241,13 @@
         <v>25</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
@@ -2229,7 +2258,7 @@
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2237,7 +2266,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F6">
         <v>9</v>
@@ -2246,13 +2275,13 @@
         <v>19</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
@@ -2263,7 +2292,7 @@
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2271,10 +2300,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F7">
         <v>9</v>
@@ -2284,7 +2313,7 @@
         <v>24.25</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -2297,7 +2326,7 @@
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -2310,7 +2339,7 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -2323,18 +2352,18 @@
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -2348,12 +2377,12 @@
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -2367,12 +2396,12 @@
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -2386,12 +2415,12 @@
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -2405,7 +2434,7 @@
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -2418,7 +2447,7 @@
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -2431,7 +2460,7 @@
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>

</xml_diff>

<commit_message>
added rogue energy logic and updated chars.xlsx
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -1,32 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593074C5-A8CE-4A3E-80D0-A6ADC49D2F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76E2EBC-4428-4D37-B143-661D7FF6E461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="212">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -226,12 +216,6 @@
     <t>DAMAGE + DEBUFF</t>
   </si>
   <si>
-    <t>SHIV</t>
-  </si>
-  <si>
-    <t>LOW DAMAGE + DEBUFF</t>
-  </si>
-  <si>
     <t>AIMED SHOT</t>
   </si>
   <si>
@@ -647,6 +631,27 @@
   </si>
   <si>
     <t>STUN, DAMAGE AND SELF HEAL</t>
+  </si>
+  <si>
+    <t>BLADE FLURRY</t>
+  </si>
+  <si>
+    <t>AOE DAMAGE DEBUFF</t>
+  </si>
+  <si>
+    <t>Choose 2nd target, that takes 50% of dmg - cannot be removed or recasted</t>
+  </si>
+  <si>
+    <t>SINISTER STRIKE</t>
+  </si>
+  <si>
+    <t>cost less energy after sinister is cast</t>
+  </si>
+  <si>
+    <t>LOCK TO TARGET</t>
+  </si>
+  <si>
+    <t>cannot change till its dead.</t>
   </si>
 </sst>
 </file>
@@ -740,14 +745,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -755,12 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -779,9 +783,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -819,9 +823,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -854,26 +858,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -906,26 +893,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1102,7 +1072,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,10 +1089,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="5"/>
       <c r="C1" t="s">
         <v>37</v>
       </c>
@@ -1138,7 +1108,7 @@
       </c>
       <c r="H1" s="7"/>
       <c r="I1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1146,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -1155,7 +1125,7 @@
         <v>58</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>65</v>
@@ -1169,39 +1139,39 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1212,13 +1182,13 @@
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>30</v>
@@ -1228,48 +1198,47 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="5"/>
       <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="5"/>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>112</v>
+      <c r="A8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1280,16 +1249,16 @@
         <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1300,13 +1269,13 @@
         <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>3</v>
@@ -1326,24 +1295,24 @@
         <v>55</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="5"/>
       <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="5"/>
       <c r="F13" t="s">
         <v>56</v>
       </c>
@@ -1357,19 +1326,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>57</v>
@@ -1380,15 +1349,15 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G15" s="1"/>
@@ -1396,16 +1365,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>60</v>
@@ -1416,10 +1385,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
@@ -1431,10 +1400,10 @@
         <v>61</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
         <v>46</v>
@@ -1446,7 +1415,7 @@
       </c>
       <c r="B19" s="7"/>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>13</v>
@@ -1465,16 +1434,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="D20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>57</v>
@@ -1485,13 +1454,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>3</v>
@@ -1501,35 +1470,35 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>31</v>
@@ -1560,16 +1529,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>3</v>
@@ -1583,45 +1552,45 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1632,13 +1601,13 @@
         <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>62</v>
@@ -1698,29 +1667,29 @@
         <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1729,10 +1698,10 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -1757,15 +1726,15 @@
       </c>
       <c r="H37" s="7"/>
       <c r="I37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>57</v>
+        <v>210</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>211</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>57</v>
@@ -1782,19 +1751,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G39" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>3</v>
@@ -1802,17 +1771,20 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F40" s="8" t="s">
+        <v>209</v>
+      </c>
       <c r="G40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1821,10 +1793,21 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F41" t="s">
+        <v>207</v>
+      </c>
       <c r="G41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1833,24 +1816,24 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="9"/>
+      <c r="B43" s="5"/>
       <c r="C43" t="s">
-        <v>146</v>
-      </c>
-      <c r="D43" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="9"/>
+      <c r="E43" s="5"/>
       <c r="F43" t="s">
-        <v>145</v>
-      </c>
-      <c r="G43" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="9"/>
+      <c r="H43" s="5"/>
       <c r="I43" t="s">
         <v>39</v>
       </c>
@@ -1877,19 +1860,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>31</v>
@@ -1897,19 +1880,19 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>31</v>
@@ -1917,36 +1900,36 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="9"/>
+      <c r="B49" s="5"/>
       <c r="C49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="9"/>
+      <c r="E49" s="5"/>
       <c r="F49" t="s">
         <v>42</v>
       </c>
@@ -1960,10 +1943,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>1</v>
@@ -1972,7 +1955,7 @@
         <v>58</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>3</v>
@@ -1980,59 +1963,59 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>31</v>
@@ -2040,32 +2023,14 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G55" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H55" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="G49:H49"/>
@@ -2075,6 +2040,24 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2100,34 +2083,34 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="E1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>178</v>
+      <c r="I1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -2138,24 +2121,24 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H2">
         <v>27</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="I2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2165,25 +2148,25 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H3">
         <f>29/2 + 16/2</f>
         <v>22.5</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
+      <c r="I3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2193,10 +2176,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F4">
         <v>13</v>
@@ -2205,19 +2188,19 @@
         <f>13+(10+14+20)/3</f>
         <v>27.666666666666664</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
+      <c r="I4" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2227,10 +2210,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -2239,23 +2222,23 @@
         <f>9+(11+14+11+28)/4</f>
         <v>25</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
+      <c r="I5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2265,7 +2248,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F6">
         <v>9</v>
@@ -2273,23 +2256,23 @@
       <c r="H6">
         <v>19</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
+      <c r="I6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2299,10 +2282,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F7">
         <v>9</v>
@@ -2311,166 +2294,166 @@
         <f>9+(0 + 9 + 13 + 9 + 9 + 9 + 9)/4</f>
         <v>23.5</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
+      <c r="I7" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H10" t="s">
-        <v>154</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
+        <v>152</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+        <v>155</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
+        <v>153</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
-      </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
+        <v>154</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
increased regen on skip
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA206F9C-3DC8-4270-905D-C47653B680A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8150C8-00CE-4A0C-90B5-D0B41216A007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="221">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -661,6 +661,24 @@
   </si>
   <si>
     <t>dot</t>
+  </si>
+  <si>
+    <t>COMPS</t>
+  </si>
+  <si>
+    <t>blessing of protection -&gt; didn’t work when target was stunned</t>
+  </si>
+  <si>
+    <t>viper sting reduces below 0</t>
+  </si>
+  <si>
+    <t>make rogues unable to skip?</t>
+  </si>
+  <si>
+    <t>no dmg</t>
+  </si>
+  <si>
+    <t>lost vs all</t>
   </si>
 </sst>
 </file>
@@ -2077,10 +2095,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2327,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -2336,15 +2354,15 @@
       </c>
       <c r="M5" s="8">
         <f>(2*I5+2*B5)/3</f>
-        <v>11.333333333333334</v>
+        <v>12.666666666666666</v>
       </c>
       <c r="N5" s="8">
         <f>(4*I5+4*B5)/5</f>
-        <v>13.6</v>
+        <v>15.2</v>
       </c>
       <c r="O5" s="8">
         <f>(9*I5+9*B5)/10</f>
-        <v>15.3</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3" t="s">
@@ -2593,6 +2611,9 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -2606,6 +2627,9 @@
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -2614,11 +2638,18 @@
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="Q11" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="S11" s="3" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -2690,9 +2721,6 @@
       <c r="V16" s="3"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -2703,7 +2731,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -2711,25 +2739,95 @@
       <c r="O18" s="9"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>205</v>
+      </c>
+      <c r="J25" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed viper sting bug
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8150C8-00CE-4A0C-90B5-D0B41216A007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3B74C6-215F-4DC1-A205-EFB33D3AD346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="228">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -675,10 +675,31 @@
     <t>make rogues unable to skip?</t>
   </si>
   <si>
-    <t>no dmg</t>
-  </si>
-  <si>
-    <t>lost vs all</t>
+    <t>WIN 3</t>
+  </si>
+  <si>
+    <t>LOSE 2</t>
+  </si>
+  <si>
+    <t>WIN 1</t>
+  </si>
+  <si>
+    <t>WIN 4</t>
+  </si>
+  <si>
+    <t>LOSE 3</t>
+  </si>
+  <si>
+    <t>WIN 5</t>
+  </si>
+  <si>
+    <t>WIN 2</t>
+  </si>
+  <si>
+    <t>LOSE 6</t>
+  </si>
+  <si>
+    <t>skipping at max mana gives you more mana than the max…</t>
   </si>
 </sst>
 </file>
@@ -779,6 +800,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,10 +816,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -1119,24 +1140,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
       <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="9"/>
       <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="9"/>
       <c r="I1" t="s">
         <v>106</v>
       </c>
@@ -1228,24 +1249,24 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="7"/>
       <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="7"/>
       <c r="F7" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="9"/>
       <c r="I7" t="s">
         <v>128</v>
       </c>
@@ -1332,24 +1353,24 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="7"/>
       <c r="F13" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="9"/>
       <c r="I13" t="s">
         <v>44</v>
       </c>
@@ -1440,24 +1461,24 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="7"/>
+      <c r="B19" s="9"/>
       <c r="C19" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="9"/>
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="7"/>
+      <c r="H19" s="9"/>
       <c r="I19" t="s">
         <v>50</v>
       </c>
@@ -1535,24 +1556,24 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="9"/>
       <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="9"/>
       <c r="F25" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="7"/>
+      <c r="H25" s="9"/>
       <c r="I25" t="s">
         <v>47</v>
       </c>
@@ -1647,24 +1668,24 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="9"/>
       <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="9"/>
       <c r="F31" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="7"/>
+      <c r="H31" s="9"/>
       <c r="I31" t="s">
         <v>38</v>
       </c>
@@ -1737,24 +1758,24 @@
       <c r="H35" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="7"/>
+      <c r="B37" s="9"/>
       <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="7"/>
+      <c r="E37" s="9"/>
       <c r="F37" t="s">
         <v>33</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="5"/>
+      <c r="H37" s="7"/>
       <c r="I37" t="s">
         <v>126</v>
       </c>
@@ -1846,24 +1867,24 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="5"/>
+      <c r="B43" s="7"/>
       <c r="C43" t="s">
         <v>145</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="5"/>
+      <c r="E43" s="7"/>
       <c r="F43" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="5"/>
+      <c r="H43" s="7"/>
       <c r="I43" t="s">
         <v>39</v>
       </c>
@@ -1949,24 +1970,24 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="5"/>
+      <c r="B49" s="7"/>
       <c r="C49" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="E49" s="7"/>
       <c r="F49" t="s">
         <v>42</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="G49" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="7"/>
+      <c r="H49" s="9"/>
       <c r="I49" t="s">
         <v>43</v>
       </c>
@@ -2061,24 +2082,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="G49:H49"/>
@@ -2088,6 +2091,24 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2095,10 +2116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2184,19 +2205,19 @@
       <c r="I2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="4">
         <f>C2</f>
         <v>30</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="4">
         <f>C2</f>
         <v>30</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="4">
         <f>C2</f>
         <v>30</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="4">
         <f>((8*C2)+2*B2)/10</f>
         <v>25.8</v>
       </c>
@@ -2237,19 +2258,19 @@
       <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="4">
         <f>(B3+C3)/2</f>
         <v>21.5</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="4">
         <f>(B3+C3*2)/3</f>
         <v>23.333333333333332</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="4">
         <f>(C3*3+2*B3)/5</f>
         <v>22.6</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="4">
         <f>(5*C3+5*B3)/10</f>
         <v>21.5</v>
       </c>
@@ -2292,19 +2313,19 @@
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="8">
+      <c r="L4" s="4">
         <f>(I4+G4)/2</f>
         <v>16</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="4">
         <f>(2*I4+G4+B4)/3</f>
         <v>18</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="4">
         <f>(4*I4+2*G4+B4)/5</f>
         <v>19.600000000000001</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="4">
         <f>(9*I4+6*B4+3*G4)/10</f>
         <v>22.8</v>
       </c>
@@ -2349,18 +2370,18 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="8">
+      <c r="L5" s="4">
         <v>10</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="4">
         <f>(2*I5+2*B5)/3</f>
         <v>12.666666666666666</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="4">
         <f>(4*I5+4*B5)/5</f>
         <v>15.2</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="4">
         <f>(9*I5+9*B5)/10</f>
         <v>17.100000000000001</v>
       </c>
@@ -2408,19 +2429,19 @@
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="8">
+      <c r="L6" s="4">
         <f>(E6+C6)/2</f>
         <v>18</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="4">
         <f>(2*I6+E6+C6)/3</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="4">
         <f>(4*I6+E6+2*C6+B6)/5</f>
         <v>17.8</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="4">
         <f>(9*I6+3*E6+4*C6+2*B6)/10</f>
         <v>20.7</v>
       </c>
@@ -2468,19 +2489,19 @@
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="8">
+      <c r="L7" s="4">
         <f>(I7+7*2)/2</f>
         <v>11.5</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="4">
         <f>(2*I7+7+G7)/3</f>
         <v>11</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="4">
         <f>((I7*4)+(G7*2)+21+B7)/5</f>
         <v>16.399999999999999</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="4">
         <f>((I7*9)+(3*G7)+(C7*2)+(2*B7)+7+7)/10</f>
         <v>17.899999999999999</v>
       </c>
@@ -2528,19 +2549,19 @@
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="8">
+      <c r="L8" s="4">
         <f>((7*2)+20)/2</f>
         <v>17</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="4">
         <f>(G8+C8+2*7)/3</f>
         <v>18.333333333333332</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="4">
         <f>(2*G8+C8+E8+7)/5</f>
         <v>17.8</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="4">
         <f>(8*I8+3*G8+2*C8+2*E8+7)/10</f>
         <v>19.100000000000001</v>
       </c>
@@ -2585,19 +2606,19 @@
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="8">
+      <c r="L9" s="4">
         <f>E9</f>
         <v>30</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="4">
         <f>(2*E9+C9)/3</f>
         <v>24.333333333333332</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="4">
         <f>(3*E9+C9+B9)/5</f>
         <v>22.6</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="4">
         <f>(5*E9+C9+4*B9)/10</f>
         <v>20.3</v>
       </c>
@@ -2617,10 +2638,10 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
@@ -2633,10 +2654,10 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3" t="s">
         <v>213</v>
@@ -2653,10 +2674,10 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
@@ -2666,10 +2687,10 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
@@ -2679,26 +2700,26 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
       <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
@@ -2709,9 +2730,9 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
@@ -2721,46 +2742,52 @@
       <c r="V16" s="3"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
       <c r="T17" s="3"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>215</v>
       </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
+      <c r="C20" t="s">
+        <v>220</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -2768,6 +2795,9 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
       <c r="J23" t="s">
         <v>216</v>
       </c>
@@ -2776,6 +2806,12 @@
       <c r="A24" t="s">
         <v>7</v>
       </c>
+      <c r="C24" t="s">
+        <v>219</v>
+      </c>
+      <c r="D24" t="s">
+        <v>224</v>
+      </c>
       <c r="J24" t="s">
         <v>217</v>
       </c>
@@ -2784,6 +2820,12 @@
       <c r="A25" t="s">
         <v>205</v>
       </c>
+      <c r="C25" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" t="s">
+        <v>226</v>
+      </c>
       <c r="J25" t="s">
         <v>218</v>
       </c>
@@ -2791,6 +2833,17 @@
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -2798,7 +2851,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
@@ -2806,7 +2859,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
@@ -2814,19 +2867,76 @@
         <v>10</v>
       </c>
     </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>4</v>
+      </c>
+    </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made rogues unable to skip
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3B74C6-215F-4DC1-A205-EFB33D3AD346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F877A70-9666-488F-B52D-BEFC14D40C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="226">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -667,12 +667,6 @@
   </si>
   <si>
     <t>blessing of protection -&gt; didn’t work when target was stunned</t>
-  </si>
-  <si>
-    <t>viper sting reduces below 0</t>
-  </si>
-  <si>
-    <t>make rogues unable to skip?</t>
   </si>
   <si>
     <t>WIN 3</t>
@@ -2082,6 +2076,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="G49:H49"/>
@@ -2091,24 +2103,6 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2119,7 +2113,7 @@
   <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2773,7 +2767,7 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -2807,13 +2801,10 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D24" t="s">
-        <v>224</v>
-      </c>
-      <c r="J24" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
@@ -2821,13 +2812,13 @@
         <v>205</v>
       </c>
       <c r="C25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J25" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
@@ -2835,10 +2826,7 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>222</v>
-      </c>
-      <c r="J26" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
@@ -2851,7 +2839,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
@@ -2859,7 +2847,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
@@ -2877,7 +2865,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -2900,7 +2888,7 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -2923,7 +2911,7 @@
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -2931,7 +2919,7 @@
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
nerfed beast hunter pet
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EEAE88-53AB-458D-B711-EAB1FA85F6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97D5A24-E4BE-4CC2-8096-2E960348E698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="227">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -690,13 +690,13 @@
     <t>LOSE 6</t>
   </si>
   <si>
-    <t>skipping at max mana gives you more mana than the max…</t>
-  </si>
-  <si>
     <t>WIN 7</t>
   </si>
   <si>
     <t>WIN 6</t>
+  </si>
+  <si>
+    <t>kc</t>
   </si>
 </sst>
 </file>
@@ -2079,6 +2079,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="G49:H49"/>
@@ -2088,24 +2106,6 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2116,7 +2116,7 @@
   <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2306,25 +2306,25 @@
         <v>2</v>
       </c>
       <c r="I4" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="4">
         <f>(I4+G4)/2</f>
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="M4" s="4">
         <f>(2*I4+G4+B4)/3</f>
-        <v>18</v>
+        <v>17.333333333333332</v>
       </c>
       <c r="N4" s="4">
-        <f>(4*I4+2*G4+B4)/5</f>
-        <v>19.600000000000001</v>
+        <f>(4*I4+2*B4+G4)/5</f>
+        <v>16.8</v>
       </c>
       <c r="O4" s="4">
         <f>(9*I4+6*B4+3*G4)/10</f>
-        <v>22.8</v>
+        <v>21.9</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
@@ -2725,9 +2725,6 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="I16" s="3"/>
-      <c r="J16" t="s">
-        <v>224</v>
-      </c>
       <c r="K16" s="3"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -2740,7 +2737,7 @@
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
@@ -2749,7 +2746,7 @@
       <c r="S17" s="5"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>215</v>
       </c>
@@ -2758,16 +2755,26 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q19" t="s">
+        <v>226</v>
+      </c>
+      <c r="U19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2779,7 +2786,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2788,17 +2795,17 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2809,7 +2816,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -2817,7 +2824,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2825,12 +2832,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2838,25 +2845,25 @@
         <v>223</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -2915,7 +2922,7 @@
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added resto druid and updated a lot of stuff
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C65D22-72F6-4701-9196-47F1DA86D7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F47F56-0562-43E3-A868-2DEC0C727609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="226">
   <si>
     <t>FROST MAGE</t>
   </si>
@@ -468,9 +468,6 @@
     <t>HOLY LIGHT</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>REJUVENATION</t>
   </si>
   <si>
@@ -688,6 +685,15 @@
   </si>
   <si>
     <t>CONSUME REJ AND/OR REG</t>
+  </si>
+  <si>
+    <t>totem instead?</t>
+  </si>
+  <si>
+    <t>INNERVATE</t>
+  </si>
+  <si>
+    <t>MANA REGEN BUFF</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1184,7 +1190,7 @@
         <v>117</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>113</v>
@@ -1353,7 +1359,7 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>11</v>
@@ -1395,7 +1401,7 @@
         <v>149</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1471,10 +1477,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>87</v>
+        <v>151</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>85</v>
@@ -1491,10 +1497,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>88</v>
@@ -1507,26 +1513,26 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>155</v>
+        <v>222</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>154</v>
+        <v>224</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>82</v>
@@ -1572,7 +1578,7 @@
         <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>223</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>100</v>
@@ -1735,7 +1741,7 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>77</v>
@@ -1768,10 +1774,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>56</v>
@@ -1794,7 +1800,7 @@
         <v>58</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>3</v>
@@ -1820,7 +1826,7 @@
         <v>3</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>123</v>
@@ -1837,13 +1843,13 @@
         <v>31</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" t="s">
         <v>177</v>
-      </c>
-      <c r="F41" t="s">
-        <v>178</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>40</v>
@@ -1897,7 +1903,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>99</v>
@@ -1980,10 +1986,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>1</v>
@@ -1992,7 +1998,7 @@
         <v>57</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>3</v>
@@ -2000,59 +2006,59 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>124</v>
       </c>
       <c r="G51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="G52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>31</v>
@@ -2060,14 +2066,32 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G55" t="s">
+        <v>172</v>
+      </c>
+      <c r="H55" t="s">
         <v>173</v>
-      </c>
-      <c r="H55" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="G49:H49"/>
@@ -2077,24 +2101,6 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2119,48 +2125,48 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s">
         <v>145</v>
       </c>
       <c r="C1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
         <v>184</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1" t="s">
         <v>187</v>
       </c>
-      <c r="E1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>189</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2209,10 +2215,10 @@
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="S2" s="3"/>
     </row>
@@ -2262,16 +2268,16 @@
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S3" s="3"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -2317,10 +2323,10 @@
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>146</v>
@@ -2328,7 +2334,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -2373,13 +2379,13 @@
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>146</v>
@@ -2387,7 +2393,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -2433,13 +2439,13 @@
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>146</v>
@@ -2456,7 +2462,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2493,21 +2499,21 @@
       </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>146</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2516,13 +2522,13 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E8">
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G8">
         <v>20</v>
@@ -2553,13 +2559,13 @@
       </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>146</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -2610,10 +2616,10 @@
       </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S9" s="3"/>
     </row>
@@ -2646,11 +2652,11 @@
       <c r="O11" s="4"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R11" s="3"/>
       <c r="S11" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
@@ -2737,7 +2743,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -2752,15 +2758,15 @@
         <v>146</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="Q19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
@@ -2768,7 +2774,7 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -2799,18 +2805,18 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -2818,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -2831,7 +2837,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -2839,7 +2845,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
@@ -2857,7 +2863,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2900,10 +2906,10 @@
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2911,7 +2917,7 @@
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2919,7 +2925,7 @@
         <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2932,12 +2938,12 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
combo points now work
</commit_message>
<xml_diff>
--- a/chars.xlsx
+++ b/chars.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B0C9B8-8DBB-4C9F-A386-A3E22873A661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D39044-DD32-4473-B572-7879C597717B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -811,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -834,7 +834,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -1141,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1492,10 +1491,10 @@
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="7"/>
       <c r="I19" t="s">
         <v>224</v>
       </c>
@@ -1519,7 +1518,7 @@
       <c r="H20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="2" t="s">
         <v>230</v>
       </c>
     </row>
@@ -1542,7 +1541,7 @@
       <c r="H21" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="2" t="s">
         <v>232</v>
       </c>
     </row>
@@ -1565,7 +1564,7 @@
       <c r="H22" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="2" t="s">
         <v>231</v>
       </c>
     </row>
@@ -1588,7 +1587,7 @@
       <c r="H23" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="2" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2119,6 +2118,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="G49:H49"/>
@@ -2128,24 +2145,6 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2155,7 +2154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>

</xml_diff>